<commit_message>
Mise a jour planning
</commit_message>
<xml_diff>
--- a/Docs/Planning.xlsx
+++ b/Docs/Planning.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tentapoulpe\Desktop\TetrisLike\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projets\Tetris\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22080" windowHeight="9636" xr2:uid="{FCFB755E-94A7-48ED-B2A9-4350E99A4DB9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22080" windowHeight="9630" xr2:uid="{FCFB755E-94A7-48ED-B2A9-4350E99A4DB9}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
+  <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,13 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
-  <si>
-    <t>Pourcentage</t>
-  </si>
-  <si>
-    <t>Deadline</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>UI :</t>
   </si>
@@ -50,9 +45,6 @@
     <t>Mécanisme de placement</t>
   </si>
   <si>
-    <t>Mécanisme de time</t>
-  </si>
-  <si>
     <t>Sélectionner</t>
   </si>
   <si>
@@ -68,9 +60,6 @@
     <t>Pause (recommencer + retour au menu principal)</t>
   </si>
   <si>
-    <t xml:space="preserve">LEVEL 1 </t>
-  </si>
-  <si>
     <t>Bouton Boutique</t>
   </si>
   <si>
@@ -87,13 +76,28 @@
   </si>
   <si>
     <t>Selection des niveaux</t>
+  </si>
+  <si>
+    <t>Poucentage</t>
+  </si>
+  <si>
+    <t>Level proto</t>
+  </si>
+  <si>
+    <t>Boutique</t>
+  </si>
+  <si>
+    <t>Mécanisme de timer</t>
+  </si>
+  <si>
+    <t>Image à reproduire</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,16 +105,50 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -118,12 +156,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -438,131 +512,227 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{839A02BB-1FC0-4FB9-92BB-8A1EC9F9563E}">
-  <dimension ref="A1:C44"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="46.5546875" customWidth="1"/>
+    <col min="1" max="1" width="46.5703125" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="2"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="B19" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="2"/>
+      <c r="E27" s="4"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B31" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="B32" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B34" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B35" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B39" s="2"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B41" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B42" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B43" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B44" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>16</v>
-      </c>
+      <c r="B45" s="5">
+        <v>0</v>
+      </c>
+      <c r="C45" s="6"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B46" s="5">
+        <v>0</v>
+      </c>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C47" s="4"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C48" s="4"/>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C49" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
actualisation du doc planning
</commit_message>
<xml_diff>
--- a/Docs/Planning.xlsx
+++ b/Docs/Planning.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projets\Tetris\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tentapoulpe\Desktop\TetrisLike\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22080" windowHeight="9630" xr2:uid="{FCFB755E-94A7-48ED-B2A9-4350E99A4DB9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22080" windowHeight="9636" xr2:uid="{FCFB755E-94A7-48ED-B2A9-4350E99A4DB9}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
   <si>
     <t>UI :</t>
   </si>
@@ -33,33 +33,12 @@
     <t>Menu (Jouer / Quitter)</t>
   </si>
   <si>
-    <t>Ecran lobby niveau + retour</t>
-  </si>
-  <si>
-    <t>Score</t>
-  </si>
-  <si>
-    <t>Mécanisme de déplacement</t>
-  </si>
-  <si>
-    <t>Mécanisme de placement</t>
-  </si>
-  <si>
-    <t>Sélectionner</t>
-  </si>
-  <si>
     <t>Prog :</t>
   </si>
   <si>
-    <t xml:space="preserve">WIN </t>
-  </si>
-  <si>
     <t>Loose</t>
   </si>
   <si>
-    <t>Pause (recommencer + retour au menu principal)</t>
-  </si>
-  <si>
     <t>Bouton Boutique</t>
   </si>
   <si>
@@ -91,13 +70,55 @@
   </si>
   <si>
     <t>Image à reproduire</t>
+  </si>
+  <si>
+    <t>Ecran lobby niveau + retour + boutique</t>
+  </si>
+  <si>
+    <t>Mécanisme de rangement</t>
+  </si>
+  <si>
+    <t>Mécanisme de tir + physique</t>
+  </si>
+  <si>
+    <t>Pause (recommencer+ retour au menu principal + boutique)</t>
+  </si>
+  <si>
+    <t>Changement de scènes</t>
+  </si>
+  <si>
+    <t>Level Design :</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Création de plusieurs niveau </t>
+  </si>
+  <si>
+    <t>Courbe de difficulté</t>
+  </si>
+  <si>
+    <t>Création de plusieurs monde</t>
+  </si>
+  <si>
+    <t>Score de fin</t>
+  </si>
+  <si>
+    <t>Scoring</t>
+  </si>
+  <si>
+    <t>3D :</t>
+  </si>
+  <si>
+    <t>Forme tetris</t>
+  </si>
+  <si>
+    <t>Mécanisme de retry</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,6 +150,15 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -188,7 +218,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -198,6 +228,11 @@
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -512,68 +547,68 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{839A02BB-1FC0-4FB9-92BB-8A1EC9F9563E}">
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="46.5703125" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="51.21875" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B1" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B9" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B10" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B17" s="2"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>1</v>
       </c>
@@ -581,140 +616,148 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="8" t="s">
         <v>2</v>
-      </c>
-      <c r="B20" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
-        <v>7</v>
       </c>
       <c r="B27" s="2"/>
       <c r="E27" s="4"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>4</v>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="9" t="s">
+        <v>17</v>
       </c>
       <c r="B29" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>5</v>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="B30" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B31" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>10</v>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="9" t="s">
+        <v>28</v>
       </c>
       <c r="B32" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>6</v>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="9" t="s">
+        <v>19</v>
       </c>
       <c r="B33" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>8</v>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="9" t="s">
+        <v>25</v>
       </c>
       <c r="B34" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B35" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B36" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B39" s="2"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
-        <v>3</v>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="9" t="s">
+        <v>24</v>
       </c>
       <c r="B41" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B42" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B43" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B44" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B44" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="B45" s="5">
         <v>0</v>
       </c>
       <c r="C45" s="6"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B46" s="5">
         <v>0</v>
@@ -722,14 +765,54 @@
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C47" s="4"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="C48" s="4"/>
     </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C49" s="4"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B50" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B51" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B52" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B57" s="12">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
actu du doc planning
</commit_message>
<xml_diff>
--- a/Docs/Planning.xlsx
+++ b/Docs/Planning.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t>UI :</t>
   </si>
@@ -112,6 +112,15 @@
   </si>
   <si>
     <t>Mécanisme de retry</t>
+  </si>
+  <si>
+    <t>DeadLine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Playtest </t>
+  </si>
+  <si>
+    <t>Prez</t>
   </si>
 </sst>
 </file>
@@ -164,7 +173,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -174,6 +183,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -218,14 +233,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -233,6 +247,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -547,10 +566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{839A02BB-1FC0-4FB9-92BB-8A1EC9F9563E}">
-  <dimension ref="A1:E57"/>
+  <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -559,47 +578,59 @@
     <col min="2" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B1" s="7" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B1" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
+      <c r="C1" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C8" s="13">
+        <v>43031</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C9" s="13">
+        <v>43031</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="3">
         <v>0</v>
       </c>
+      <c r="C10" s="13">
+        <v>43031</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B17" s="2"/>
@@ -615,22 +646,28 @@
       <c r="B19" s="3">
         <v>0</v>
       </c>
+      <c r="C19" s="13">
+        <v>43028</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B20" s="3">
         <v>0</v>
       </c>
+      <c r="C20" s="13">
+        <v>43028</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="13" t="s">
+      <c r="A25" s="12" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="8" t="s">
+      <c r="A27" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B27" s="2"/>
@@ -641,19 +678,25 @@
       <c r="B28" s="2"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="9" t="s">
+      <c r="A29" s="8" t="s">
         <v>17</v>
       </c>
       <c r="B29" s="3">
         <v>0</v>
       </c>
+      <c r="C29" s="13">
+        <v>43028</v>
+      </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="9" t="s">
+      <c r="A30" s="8" t="s">
         <v>16</v>
       </c>
       <c r="B30" s="3">
         <v>0</v>
+      </c>
+      <c r="C30" s="13">
+        <v>43028</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -663,29 +706,41 @@
       <c r="B31" s="3">
         <v>0</v>
       </c>
+      <c r="C31" s="13">
+        <v>43032</v>
+      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="9" t="s">
+      <c r="A32" s="8" t="s">
         <v>28</v>
       </c>
       <c r="B32" s="3">
         <v>0</v>
       </c>
+      <c r="C32" s="13">
+        <v>43033</v>
+      </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="9" t="s">
+      <c r="A33" s="8" t="s">
         <v>19</v>
       </c>
       <c r="B33" s="3">
         <v>0</v>
       </c>
+      <c r="C33" s="13">
+        <v>43028</v>
+      </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="9" t="s">
+      <c r="A34" s="8" t="s">
         <v>25</v>
       </c>
       <c r="B34" s="3">
         <v>0</v>
+      </c>
+      <c r="C34" s="13">
+        <v>43032</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -695,17 +750,23 @@
       <c r="B35" s="3">
         <v>0</v>
       </c>
+      <c r="C35" s="13">
+        <v>43032</v>
+      </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B36" s="12">
-        <v>0</v>
+      <c r="B36" s="11">
+        <v>0</v>
+      </c>
+      <c r="C36" s="13">
+        <v>43033</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="8" t="s">
+      <c r="A39" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B39" s="2"/>
@@ -715,19 +776,25 @@
       <c r="B40" s="2"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="9" t="s">
+      <c r="A41" s="8" t="s">
         <v>24</v>
       </c>
       <c r="B41" s="3">
         <v>0</v>
       </c>
+      <c r="C41" s="13">
+        <v>43031</v>
+      </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="2" t="s">
+      <c r="A42" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B42" s="3">
         <v>0</v>
+      </c>
+      <c r="C42" s="13">
+        <v>43031</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
@@ -737,6 +804,9 @@
       <c r="B43" s="3">
         <v>0</v>
       </c>
+      <c r="C43" s="13">
+        <v>43031</v>
+      </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
@@ -745,6 +815,9 @@
       <c r="B44" s="3">
         <v>0</v>
       </c>
+      <c r="C44" s="13">
+        <v>43031</v>
+      </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
@@ -753,7 +826,12 @@
       <c r="B45" s="5">
         <v>0</v>
       </c>
-      <c r="C45" s="6"/>
+      <c r="C45" s="16">
+        <v>43031</v>
+      </c>
+      <c r="D45" s="13">
+        <v>43031</v>
+      </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
@@ -762,14 +840,16 @@
       <c r="B46" s="5">
         <v>0</v>
       </c>
-      <c r="C46" s="4"/>
+      <c r="C46" s="15">
+        <v>43028</v>
+      </c>
       <c r="D46" s="4"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C47" s="4"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="7" t="s">
+      <c r="A48" s="6" t="s">
         <v>20</v>
       </c>
       <c r="C48" s="4"/>
@@ -778,41 +858,78 @@
       <c r="C49" s="4"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" s="11" t="s">
+      <c r="A50" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B50" s="12">
-        <v>0</v>
+      <c r="B50" s="11">
+        <v>0</v>
+      </c>
+      <c r="C50" s="13">
+        <v>43021</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51" s="11" t="s">
+      <c r="A51" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B51" s="12">
-        <v>0</v>
+      <c r="B51" s="11">
+        <v>0</v>
+      </c>
+      <c r="C51" s="14">
+        <v>43021</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A52" s="11" t="s">
+      <c r="A52" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B52" s="12">
-        <v>0</v>
+      <c r="B52" s="11">
+        <v>0</v>
+      </c>
+      <c r="C52" s="13">
+        <v>43021</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A55" s="7" t="s">
+      <c r="A55" s="6" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A57" s="10" t="s">
+      <c r="A57" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B57" s="12">
-        <v>0</v>
-      </c>
+      <c r="B57" s="11">
+        <v>0</v>
+      </c>
+      <c r="C57" s="13">
+        <v>43028</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B59" s="11">
+        <v>0</v>
+      </c>
+      <c r="C59" s="13">
+        <v>43033</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B60" s="11">
+        <v>0</v>
+      </c>
+      <c r="C60" s="13">
+        <v>43034</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B61" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
actu planning encore ....
</commit_message>
<xml_diff>
--- a/Docs/Planning.xlsx
+++ b/Docs/Planning.xlsx
@@ -42,9 +42,6 @@
     <t>Bouton Boutique</t>
   </si>
   <si>
-    <t>Bouton Pause (reprendre + recommencer quitter)</t>
-  </si>
-  <si>
     <t>Menu (Jouer/Quitter)</t>
   </si>
   <si>
@@ -120,7 +117,10 @@
     <t>Interface (cadre)</t>
   </si>
   <si>
-    <t>Pause</t>
+    <t xml:space="preserve">Bouton Pause </t>
+  </si>
+  <si>
+    <t>Pause (reprendre + recommencer quitter)</t>
   </si>
 </sst>
 </file>
@@ -557,8 +557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D55" sqref="D55"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -569,10 +569,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -587,7 +587,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="5">
         <v>0</v>
@@ -598,7 +598,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" s="5">
         <v>0</v>
@@ -609,7 +609,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" s="5">
         <v>0</v>
@@ -641,7 +641,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B20" s="5">
         <v>0</v>
@@ -652,7 +652,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -668,7 +668,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B29" s="5">
         <v>0</v>
@@ -679,7 +679,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B30" s="5">
         <v>0</v>
@@ -690,7 +690,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B31" s="5">
         <v>0</v>
@@ -701,7 +701,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B32" s="5">
         <v>0</v>
@@ -712,7 +712,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B33" s="5">
         <v>0</v>
@@ -723,7 +723,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B34" s="5">
         <v>0</v>
@@ -745,7 +745,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B36" s="9">
         <v>0</v>
@@ -766,7 +766,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B41" s="5">
         <v>0</v>
@@ -777,7 +777,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="B42" s="5">
         <v>0</v>
@@ -799,7 +799,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B44" s="5">
         <v>0</v>
@@ -810,7 +810,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B45" s="10">
         <v>0</v>
@@ -836,7 +836,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C48" s="8"/>
     </row>
@@ -845,7 +845,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B50" s="9">
         <v>0</v>
@@ -856,7 +856,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B51" s="9">
         <v>0</v>
@@ -867,7 +867,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B52" s="9">
         <v>0</v>
@@ -878,12 +878,12 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B57" s="9">
         <v>0</v>
@@ -894,7 +894,7 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B59" s="9">
         <v>0</v>
@@ -905,7 +905,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B60" s="9">
         <v>0</v>

</xml_diff>

<commit_message>
Actu planning musiques et sons
</commit_message>
<xml_diff>
--- a/Docs/Planning.xlsx
+++ b/Docs/Planning.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
   <si>
     <t>UI :</t>
   </si>
@@ -121,14 +121,43 @@
   </si>
   <si>
     <t>Pause (reprendre + recommencer quitter)</t>
+  </si>
+  <si>
+    <t>Son :</t>
+  </si>
+  <si>
+    <t>Musique d'écran d'accueil</t>
+  </si>
+  <si>
+    <t>Effets sonores boutons</t>
+  </si>
+  <si>
+    <t>Effets sonores boutons pause et boutique</t>
+  </si>
+  <si>
+    <t>Musique Monde 1</t>
+  </si>
+  <si>
+    <t>Effet sonore de grab</t>
+  </si>
+  <si>
+    <t>Effet sonore de rangement</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -226,21 +255,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -555,367 +585,432 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E61"/>
+  <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="51.33203125" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="11.44140625" style="1"/>
+    <col min="1" max="1" width="51.33203125" style="2" customWidth="1"/>
+    <col min="2" max="16384" width="11.44140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="4"/>
+      <c r="B6" s="5"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="5">
-        <v>0</v>
-      </c>
-      <c r="C8" s="6">
+      <c r="B8" s="6">
+        <v>0</v>
+      </c>
+      <c r="C8" s="7">
         <v>43031</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="5">
-        <v>0</v>
-      </c>
-      <c r="C9" s="6">
+      <c r="B9" s="6">
+        <v>0</v>
+      </c>
+      <c r="C9" s="7">
         <v>43031</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="5">
-        <v>0</v>
-      </c>
-      <c r="C10" s="6">
+      <c r="B10" s="6">
+        <v>0</v>
+      </c>
+      <c r="C10" s="7">
         <v>43031</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B17" s="4"/>
+      <c r="A17" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="5"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="5">
-        <v>0</v>
-      </c>
-      <c r="C19" s="6">
+      <c r="B19" s="6">
+        <v>0</v>
+      </c>
+      <c r="C19" s="7">
         <v>43028</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="5">
-        <v>0</v>
-      </c>
-      <c r="C20" s="6">
+      <c r="B20" s="6">
+        <v>0</v>
+      </c>
+      <c r="C20" s="7">
         <v>43028</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="8" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B27" s="4"/>
-      <c r="E27" s="8"/>
+      <c r="B27" s="5"/>
+      <c r="E27" s="9"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="5">
-        <v>0</v>
-      </c>
-      <c r="C29" s="6">
+      <c r="B29" s="6">
+        <v>0</v>
+      </c>
+      <c r="C29" s="7">
         <v>43028</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B30" s="5">
-        <v>0</v>
-      </c>
-      <c r="C30" s="6">
+      <c r="B30" s="6">
+        <v>0</v>
+      </c>
+      <c r="C30" s="7">
         <v>43028</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="4" t="s">
+      <c r="A31" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B31" s="5">
-        <v>0</v>
-      </c>
-      <c r="C31" s="6">
+      <c r="B31" s="6">
+        <v>0</v>
+      </c>
+      <c r="C31" s="7">
         <v>43032</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B32" s="5">
-        <v>0</v>
-      </c>
-      <c r="C32" s="6">
+      <c r="B32" s="6">
+        <v>0</v>
+      </c>
+      <c r="C32" s="7">
         <v>43033</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="4" t="s">
+      <c r="A33" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B33" s="5">
-        <v>0</v>
-      </c>
-      <c r="C33" s="6">
+      <c r="B33" s="6">
+        <v>0</v>
+      </c>
+      <c r="C33" s="7">
         <v>43028</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="4" t="s">
+      <c r="A34" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B34" s="5">
-        <v>0</v>
-      </c>
-      <c r="C34" s="6">
+      <c r="B34" s="6">
+        <v>0</v>
+      </c>
+      <c r="C34" s="7">
         <v>43032</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="4" t="s">
+      <c r="A35" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B35" s="5">
-        <v>0</v>
-      </c>
-      <c r="C35" s="6">
+      <c r="B35" s="6">
+        <v>0</v>
+      </c>
+      <c r="C35" s="7">
         <v>43032</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
+      <c r="A36" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B36" s="9">
-        <v>0</v>
-      </c>
-      <c r="C36" s="6">
+      <c r="B36" s="10">
+        <v>0</v>
+      </c>
+      <c r="C36" s="7">
         <v>43033</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B39" s="4"/>
+      <c r="A39" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B39" s="5"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="4"/>
-      <c r="B40" s="4"/>
+      <c r="A40" s="5"/>
+      <c r="B40" s="5"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="4" t="s">
+      <c r="A41" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B41" s="5">
-        <v>0</v>
-      </c>
-      <c r="C41" s="6">
+      <c r="B41" s="6">
+        <v>0</v>
+      </c>
+      <c r="C41" s="7">
         <v>43031</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="4" t="s">
+      <c r="A42" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B42" s="5">
-        <v>0</v>
-      </c>
-      <c r="C42" s="6">
+      <c r="B42" s="6">
+        <v>0</v>
+      </c>
+      <c r="C42" s="7">
         <v>43028</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="4" t="s">
+      <c r="A43" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B43" s="5">
-        <v>0</v>
-      </c>
-      <c r="C43" s="6">
+      <c r="B43" s="6">
+        <v>0</v>
+      </c>
+      <c r="C43" s="7">
         <v>43028</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="4" t="s">
+      <c r="A44" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B44" s="5">
-        <v>0</v>
-      </c>
-      <c r="C44" s="6">
+      <c r="B44" s="6">
+        <v>0</v>
+      </c>
+      <c r="C44" s="7">
         <v>43028</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="4" t="s">
+      <c r="A45" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B45" s="10">
-        <v>0</v>
-      </c>
-      <c r="C45" s="6">
+      <c r="B45" s="11">
+        <v>0</v>
+      </c>
+      <c r="C45" s="7">
         <v>43031</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="4" t="s">
+      <c r="A46" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B46" s="10">
-        <v>0</v>
-      </c>
-      <c r="C46" s="11">
+      <c r="B46" s="11">
+        <v>0</v>
+      </c>
+      <c r="C46" s="12">
         <v>43031</v>
       </c>
-      <c r="D46" s="8"/>
+      <c r="D46" s="9"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C47" s="8"/>
+      <c r="C47" s="9"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="2" t="s">
+      <c r="A48" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C48" s="8"/>
+      <c r="C48" s="9"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C49" s="8"/>
+      <c r="C49" s="9"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" s="12" t="s">
+      <c r="A50" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B50" s="9">
-        <v>0</v>
-      </c>
-      <c r="C50" s="6">
+      <c r="B50" s="10">
+        <v>0</v>
+      </c>
+      <c r="C50" s="7">
         <v>43031</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51" s="12" t="s">
+      <c r="A51" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B51" s="9">
-        <v>0</v>
-      </c>
-      <c r="C51" s="6">
+      <c r="B51" s="10">
+        <v>0</v>
+      </c>
+      <c r="C51" s="7">
         <v>43031</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A52" s="12" t="s">
+      <c r="A52" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B52" s="9">
-        <v>0</v>
-      </c>
-      <c r="C52" s="6">
+      <c r="B52" s="10">
+        <v>0</v>
+      </c>
+      <c r="C52" s="7">
         <v>43031</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A55" s="2" t="s">
+      <c r="A55" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A57" s="1" t="s">
+      <c r="A57" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B57" s="9">
-        <v>0</v>
-      </c>
-      <c r="C57" s="6">
+      <c r="B57" s="10">
+        <v>0</v>
+      </c>
+      <c r="C57" s="7">
         <v>43032</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A59" s="1" t="s">
+      <c r="A59" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B59" s="9">
-        <v>0</v>
-      </c>
-      <c r="C59" s="6">
+      <c r="B59" s="10">
+        <v>0</v>
+      </c>
+      <c r="C59" s="7">
         <v>43033</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A60" s="1" t="s">
+      <c r="A60" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B60" s="9">
-        <v>0</v>
-      </c>
-      <c r="C60" s="6">
+      <c r="B60" s="10">
+        <v>0</v>
+      </c>
+      <c r="C60" s="7">
         <v>43034</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B61" s="13"/>
+      <c r="B61" s="14"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B65" s="10">
+        <v>0</v>
+      </c>
+      <c r="C65" s="7">
+        <v>43033</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B66" s="10">
+        <v>0</v>
+      </c>
+      <c r="C66" s="7">
+        <v>43033</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B67" s="10">
+        <v>0</v>
+      </c>
+      <c r="C67" s="7">
+        <v>43033</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B68" s="10">
+        <v>0</v>
+      </c>
+      <c r="C68" s="7">
+        <v>43033</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B69" s="10">
+        <v>0</v>
+      </c>
+      <c r="C69" s="7">
+        <v>43033</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" s="2" t="s">
+        <v>38</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
folder prefabs + prefab menu pause et menu principal
</commit_message>
<xml_diff>
--- a/Docs/Planning.xlsx
+++ b/Docs/Planning.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tentapoulpe\Desktop\TetrisLike\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louis\Desktop\tetris\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
   <si>
     <t>Pourcentage</t>
   </si>
@@ -101,9 +101,6 @@
     <t>Score</t>
   </si>
   <si>
-    <t>Pause (Recommencer + Quitter + Continuer + boutique)</t>
-  </si>
-  <si>
     <t>Fenetre de fin (score + recommencer + retour au menu)</t>
   </si>
   <si>
@@ -150,13 +147,26 @@
   </si>
   <si>
     <t>Musique Monde 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boutique </t>
+  </si>
+  <si>
+    <t>Pause (Recommencer + Quitter + Continuer)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -166,6 +176,7 @@
     </font>
     <font>
       <b/>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -174,7 +185,6 @@
     </font>
     <font>
       <b/>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -222,13 +232,13 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -545,428 +555,440 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5A1332F-9C89-4503-92BB-2BAE5CF2A291}">
   <dimension ref="A1:C68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C68" sqref="C68"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="50" customWidth="1"/>
+    <col min="1" max="1" width="50" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="1">
-        <v>0</v>
-      </c>
-      <c r="C9" s="7">
+      <c r="B9" s="4">
+        <v>0</v>
+      </c>
+      <c r="C9" s="5">
         <v>43031</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="1">
-        <v>0</v>
-      </c>
-      <c r="C10" s="7">
+      <c r="B10" s="4">
+        <v>0</v>
+      </c>
+      <c r="C10" s="5">
         <v>43032</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="1">
-        <v>0</v>
-      </c>
-      <c r="C11" s="7">
+      <c r="B11" s="4">
+        <v>0</v>
+      </c>
+      <c r="C11" s="5">
         <v>43032</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="1">
-        <v>0</v>
-      </c>
-      <c r="C12" s="7">
+      <c r="B12" s="4">
+        <v>0</v>
+      </c>
+      <c r="C12" s="5">
         <v>43031</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="A18" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="1">
-        <v>0</v>
-      </c>
-      <c r="C18" s="7">
+      <c r="B18" s="4">
+        <v>0</v>
+      </c>
+      <c r="C18" s="5">
         <v>43028</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="A19" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="2">
-        <v>0</v>
-      </c>
-      <c r="C19" s="7">
+      <c r="B19" s="4">
+        <v>0</v>
+      </c>
+      <c r="C19" s="5">
         <v>43032</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="A20" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="1">
-        <v>0</v>
-      </c>
-      <c r="C20" s="7">
+      <c r="B20" s="4">
+        <v>0</v>
+      </c>
+      <c r="C20" s="5">
         <v>43031</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="5" t="s">
+      <c r="A26" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+      <c r="A28" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" s="4">
+        <v>0</v>
+      </c>
+      <c r="C28" s="5">
+        <v>43028</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="6">
+        <v>1</v>
+      </c>
+      <c r="C29" s="5">
+        <v>43028</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B30" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="C30" s="5">
+        <v>43028</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B31" s="4">
+        <v>0</v>
+      </c>
+      <c r="C31" s="5">
+        <v>43028</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32" s="4">
+        <v>0</v>
+      </c>
+      <c r="C32" s="5">
+        <v>43028</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B33" s="4">
+        <v>0</v>
+      </c>
+      <c r="C33" s="5">
+        <v>43028</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B34" s="4">
+        <v>0</v>
+      </c>
+      <c r="C34" s="5">
+        <v>43031</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B35" s="4">
+        <v>0</v>
+      </c>
+      <c r="C35" s="5">
+        <v>43032</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B36" s="4">
+        <v>0</v>
+      </c>
+      <c r="C36" s="5">
+        <v>43031</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B37" s="4">
+        <v>0</v>
+      </c>
+      <c r="C37" s="5">
+        <v>43028</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B38" s="4">
+        <v>0</v>
+      </c>
+      <c r="C38" s="5">
+        <v>43028</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B39" s="4">
+        <v>0</v>
+      </c>
+      <c r="C39" s="5">
+        <v>43028</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B28" s="1">
-        <v>0</v>
-      </c>
-      <c r="C28" s="7">
-        <v>43028</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>13</v>
-      </c>
-      <c r="B29" s="4">
+      <c r="B40" s="4">
+        <v>0</v>
+      </c>
+      <c r="C40" s="5">
+        <v>43028</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B44" s="4">
+        <v>0</v>
+      </c>
+      <c r="C44" s="5">
+        <v>43028</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B45" s="4">
+        <v>0</v>
+      </c>
+      <c r="C45" s="5">
+        <v>43028</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B46" s="6">
         <v>1</v>
       </c>
-      <c r="C29" s="7">
-        <v>43028</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>14</v>
-      </c>
-      <c r="B30" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="C30" s="7">
-        <v>43028</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>15</v>
-      </c>
-      <c r="B31" s="1">
-        <v>0</v>
-      </c>
-      <c r="C31" s="7">
-        <v>43028</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>16</v>
-      </c>
-      <c r="B32" s="1">
-        <v>0</v>
-      </c>
-      <c r="C32" s="7">
-        <v>43028</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>18</v>
-      </c>
-      <c r="B33" s="1">
-        <v>0</v>
-      </c>
-      <c r="C33" s="7">
-        <v>43028</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>17</v>
-      </c>
-      <c r="B34" s="1">
-        <v>0</v>
-      </c>
-      <c r="C34" s="7">
-        <v>43031</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>19</v>
-      </c>
-      <c r="B35" s="1">
-        <v>0</v>
-      </c>
-      <c r="C35" s="7">
+      <c r="C46" s="5">
+        <v>43028</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B47" s="4">
+        <v>0</v>
+      </c>
+      <c r="C47" s="5">
+        <v>43028</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B48" s="4">
+        <v>0</v>
+      </c>
+      <c r="C48" s="5">
+        <v>43028</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B54" s="4">
+        <v>0</v>
+      </c>
+      <c r="C54" s="5">
+        <v>43033</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B55" s="4">
+        <v>0</v>
+      </c>
+      <c r="C55" s="5">
+        <v>43033</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B59" s="6">
+        <v>1</v>
+      </c>
+      <c r="C59" s="5">
+        <v>43028</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B63" s="4">
+        <v>0</v>
+      </c>
+      <c r="C63" s="5">
         <v>43032</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>20</v>
-      </c>
-      <c r="B36" s="1">
-        <v>0</v>
-      </c>
-      <c r="C36" s="7">
-        <v>43031</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>21</v>
-      </c>
-      <c r="B37" s="1">
-        <v>0</v>
-      </c>
-      <c r="C37" s="7">
-        <v>43028</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>22</v>
-      </c>
-      <c r="B38" s="1">
-        <v>0</v>
-      </c>
-      <c r="C38" s="7">
-        <v>43028</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B64" s="4">
+        <v>0</v>
+      </c>
+      <c r="C64" s="5">
+        <v>43032</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B65" s="4">
+        <v>0</v>
+      </c>
+      <c r="C65" s="5">
+        <v>43032</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B39" s="1">
-        <v>0</v>
-      </c>
-      <c r="C39" s="7">
-        <v>43028</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>39</v>
-      </c>
-      <c r="B40" s="1">
-        <v>0</v>
-      </c>
-      <c r="C40" s="7">
-        <v>43028</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>23</v>
-      </c>
-      <c r="B44" s="1">
-        <v>0</v>
-      </c>
-      <c r="C44" s="7">
-        <v>43028</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>25</v>
-      </c>
-      <c r="B45" s="1">
-        <v>0</v>
-      </c>
-      <c r="C45" s="7">
-        <v>43028</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>24</v>
-      </c>
-      <c r="B46" s="4">
-        <v>1</v>
-      </c>
-      <c r="C46" s="7">
-        <v>43028</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>26</v>
-      </c>
-      <c r="B47" s="1">
-        <v>0</v>
-      </c>
-      <c r="C47" s="7">
-        <v>43028</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A52" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>28</v>
-      </c>
-      <c r="B54" s="1">
-        <v>0</v>
-      </c>
-      <c r="C54" s="7">
-        <v>43033</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>29</v>
-      </c>
-      <c r="B55" s="1">
-        <v>0</v>
-      </c>
-      <c r="C55" s="7">
-        <v>43033</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
-        <v>31</v>
-      </c>
-      <c r="B59" s="4">
-        <v>1</v>
-      </c>
-      <c r="C59" s="7">
-        <v>43028</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A61" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
-        <v>33</v>
-      </c>
-      <c r="B63" s="1">
-        <v>0</v>
-      </c>
-      <c r="C63" s="7">
+      <c r="B66" s="4">
+        <v>0</v>
+      </c>
+      <c r="C66" s="5">
         <v>43032</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B64" s="1">
-        <v>0</v>
-      </c>
-      <c r="C64" s="7">
+      <c r="B67" s="4">
+        <v>0</v>
+      </c>
+      <c r="C67" s="5">
         <v>43032</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
-        <v>37</v>
-      </c>
-      <c r="B65" s="1">
-        <v>0</v>
-      </c>
-      <c r="C65" s="7">
-        <v>43032</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
-        <v>41</v>
-      </c>
-      <c r="B66" s="1">
-        <v>0</v>
-      </c>
-      <c r="C66" s="7">
-        <v>43032</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B67" s="1">
-        <v>0</v>
-      </c>
-      <c r="C67" s="7">
-        <v>43032</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
-        <v>36</v>
-      </c>
-      <c r="B68" s="1">
-        <v>0</v>
-      </c>
-      <c r="C68" s="7">
+      <c r="B68" s="4">
+        <v>0</v>
+      </c>
+      <c r="C68" s="5">
         <v>43032</v>
       </c>
     </row>

</xml_diff>

<commit_message>
maj planning + script mur
</commit_message>
<xml_diff>
--- a/Docs/Planning.xlsx
+++ b/Docs/Planning.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louis\Desktop\tetris\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tentapoulpe\Desktop\TetrisLike\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -555,8 +555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5A1332F-9C89-4503-92BB-2BAE5CF2A291}">
   <dimension ref="A1:C68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -587,8 +587,8 @@
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="4">
-        <v>0</v>
+      <c r="B9" s="6">
+        <v>1</v>
       </c>
       <c r="C9" s="5">
         <v>43031</v>
@@ -598,8 +598,8 @@
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="4">
-        <v>0</v>
+      <c r="B10" s="6">
+        <v>1</v>
       </c>
       <c r="C10" s="5">
         <v>43032</v>
@@ -609,8 +609,8 @@
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="4">
-        <v>0</v>
+      <c r="B11" s="6">
+        <v>1</v>
       </c>
       <c r="C11" s="5">
         <v>43032</v>
@@ -712,8 +712,8 @@
       <c r="A31" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B31" s="4">
-        <v>0</v>
+      <c r="B31" s="6">
+        <v>1</v>
       </c>
       <c r="C31" s="5">
         <v>43028</v>
@@ -734,8 +734,8 @@
       <c r="A33" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B33" s="4">
-        <v>0</v>
+      <c r="B33" s="7">
+        <v>0.8</v>
       </c>
       <c r="C33" s="5">
         <v>43028</v>
@@ -778,8 +778,8 @@
       <c r="A37" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B37" s="4">
-        <v>0</v>
+      <c r="B37" s="7">
+        <v>0.2</v>
       </c>
       <c r="C37" s="5">
         <v>43028</v>
@@ -850,7 +850,7 @@
         <v>24</v>
       </c>
       <c r="B46" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C46" s="5">
         <v>43028</v>

</xml_diff>

<commit_message>
mise a jour planning + script holes
</commit_message>
<xml_diff>
--- a/Docs/Planning.xlsx
+++ b/Docs/Planning.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="48">
   <si>
     <t>Pourcentage</t>
   </si>
@@ -149,10 +149,25 @@
     <t>Musique Monde 1</t>
   </si>
   <si>
-    <t xml:space="preserve">Boutique </t>
-  </si>
-  <si>
     <t>Pause (Recommencer + Quitter + Continuer)</t>
+  </si>
+  <si>
+    <t>a verifier panel pour desactiver le drag</t>
+  </si>
+  <si>
+    <t>Micka</t>
+  </si>
+  <si>
+    <t>Arthur</t>
+  </si>
+  <si>
+    <t>Louis</t>
+  </si>
+  <si>
+    <t>Tous</t>
+  </si>
+  <si>
+    <t>Kevin/jyjy</t>
   </si>
 </sst>
 </file>
@@ -192,7 +207,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -217,6 +232,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -230,15 +251,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -553,16 +575,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5A1332F-9C89-4503-92BB-2BAE5CF2A291}">
-  <dimension ref="A1:C68"/>
+  <dimension ref="A1:D68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="50" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="11.5546875" style="1"/>
+    <col min="2" max="3" width="11.5546875" style="1"/>
+    <col min="4" max="4" width="35.109375" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -587,7 +611,7 @@
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="4">
         <v>1</v>
       </c>
       <c r="C9" s="5">
@@ -598,7 +622,7 @@
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="4">
         <v>1</v>
       </c>
       <c r="C10" s="5">
@@ -609,7 +633,7 @@
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="4">
         <v>1</v>
       </c>
       <c r="C11" s="5">
@@ -621,7 +645,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12" s="5">
         <v>43031</v>
@@ -632,220 +656,250 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B18" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C18" s="5">
         <v>43028</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B19" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C19" s="5">
         <v>43032</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B20" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C20" s="5">
         <v>43031</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B28" s="4">
+      <c r="B28" s="6">
         <v>0</v>
       </c>
       <c r="C28" s="5">
         <v>43028</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D28" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B29" s="6">
+      <c r="B29" s="4">
         <v>1</v>
       </c>
       <c r="C29" s="5">
         <v>43028</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B30" s="7">
-        <v>0.8</v>
+      <c r="B30" s="4">
+        <v>1</v>
       </c>
       <c r="C30" s="5">
         <v>43028</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B31" s="6">
+      <c r="B31" s="4">
         <v>1</v>
       </c>
       <c r="C31" s="5">
         <v>43028</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B32" s="4">
+      <c r="B32" s="6">
         <v>0</v>
       </c>
       <c r="C32" s="5">
         <v>43028</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D32" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B33" s="7">
-        <v>0.8</v>
+      <c r="B33" s="4">
+        <v>1</v>
       </c>
       <c r="C33" s="5">
         <v>43028</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D33" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B34" s="4">
+      <c r="B34" s="6">
         <v>0</v>
       </c>
       <c r="C34" s="5">
         <v>43031</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D34" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B35" s="4">
+      <c r="B35" s="6">
         <v>0</v>
       </c>
       <c r="C35" s="5">
         <v>43032</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D35" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B36" s="4">
+      <c r="B36" s="6">
         <v>0</v>
       </c>
       <c r="C36" s="5">
         <v>43031</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D36" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B37" s="7">
-        <v>0.2</v>
+        <v>0.9</v>
       </c>
       <c r="C37" s="5">
         <v>43028</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D37" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B38" s="4">
+      <c r="B38" s="6">
         <v>0</v>
       </c>
       <c r="C38" s="5">
         <v>43028</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D38" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B39" s="4">
+      <c r="B39" s="6">
         <v>0</v>
       </c>
       <c r="C39" s="5">
         <v>43028</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D39" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B40" s="4">
+      <c r="B40" s="6">
         <v>0</v>
       </c>
       <c r="C40" s="5">
         <v>43028</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D40" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B44" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C44" s="5">
         <v>43028</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B45" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C45" s="5">
         <v>43028</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>24</v>
       </c>
@@ -855,141 +909,161 @@
       <c r="C46" s="5">
         <v>43028</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D46" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B47" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C47" s="5">
         <v>43028</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A48" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B48" s="4">
-        <v>0</v>
-      </c>
-      <c r="C48" s="5">
-        <v>43028</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B48" s="8"/>
+      <c r="C48" s="5"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B54" s="4">
+      <c r="B54" s="6">
         <v>0</v>
       </c>
       <c r="C54" s="5">
         <v>43033</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D54" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B55" s="4">
+      <c r="B55" s="6">
         <v>0</v>
       </c>
       <c r="C55" s="5">
         <v>43033</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D55" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B59" s="6">
+      <c r="B59" s="4">
         <v>1</v>
       </c>
       <c r="C59" s="5">
         <v>43028</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B63" s="4">
+      <c r="B63" s="6">
         <v>0</v>
       </c>
       <c r="C63" s="5">
         <v>43032</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D63" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B64" s="4">
+      <c r="B64" s="6">
         <v>0</v>
       </c>
       <c r="C64" s="5">
         <v>43032</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D64" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B65" s="4">
+      <c r="B65" s="6">
         <v>0</v>
       </c>
       <c r="C65" s="5">
         <v>43032</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D65" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B66" s="4">
+      <c r="B66" s="6">
         <v>0</v>
       </c>
       <c r="C66" s="5">
         <v>43032</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D66" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B67" s="4">
+      <c r="B67" s="6">
         <v>0</v>
       </c>
       <c r="C67" s="5">
         <v>43032</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D67" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B68" s="4">
+      <c r="B68" s="6">
         <v>0</v>
       </c>
       <c r="C68" s="5">
         <v>43032</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
maj planning + script arthur
</commit_message>
<xml_diff>
--- a/Docs/Planning.xlsx
+++ b/Docs/Planning.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="48">
   <si>
     <t>Pourcentage</t>
   </si>
@@ -92,9 +92,6 @@
     <t>Prochaine scène (mur)</t>
   </si>
   <si>
-    <t>Scoring</t>
-  </si>
-  <si>
     <t>Interface in-game</t>
   </si>
   <si>
@@ -168,6 +165,9 @@
   </si>
   <si>
     <t>Kevin/jyjy</t>
+  </si>
+  <si>
+    <t>Scoring + timer</t>
   </si>
 </sst>
 </file>
@@ -577,8 +577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5A1332F-9C89-4503-92BB-2BAE5CF2A291}">
   <dimension ref="A1:D68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -701,7 +701,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B28" s="6">
         <v>0</v>
@@ -710,7 +710,7 @@
         <v>43028</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -750,14 +750,11 @@
       <c r="A32" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B32" s="6">
-        <v>0</v>
+      <c r="B32" s="4">
+        <v>1</v>
       </c>
       <c r="C32" s="5">
         <v>43028</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -771,7 +768,7 @@
         <v>43028</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -785,7 +782,7 @@
         <v>43031</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -799,7 +796,7 @@
         <v>43032</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
@@ -813,7 +810,7 @@
         <v>43031</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
@@ -827,12 +824,12 @@
         <v>43028</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="B38" s="6">
         <v>0</v>
@@ -841,12 +838,12 @@
         <v>43028</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B39" s="6">
         <v>0</v>
@@ -855,12 +852,12 @@
         <v>43028</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B40" s="6">
         <v>0</v>
@@ -869,7 +866,7 @@
         <v>43028</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
@@ -879,7 +876,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B44" s="4">
         <v>1</v>
@@ -890,7 +887,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B45" s="4">
         <v>1</v>
@@ -901,21 +898,18 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B46" s="6">
-        <v>0</v>
+        <v>23</v>
+      </c>
+      <c r="B46" s="4">
+        <v>1</v>
       </c>
       <c r="C46" s="5">
         <v>43028</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B47" s="4">
         <v>1</v>
@@ -930,12 +924,12 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B54" s="6">
         <v>0</v>
@@ -944,12 +938,12 @@
         <v>43033</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B55" s="6">
         <v>0</v>
@@ -958,17 +952,17 @@
         <v>43033</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B59" s="4">
         <v>1</v>
@@ -979,12 +973,12 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B63" s="6">
         <v>0</v>
@@ -993,12 +987,12 @@
         <v>43032</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B64" s="6">
         <v>0</v>
@@ -1007,12 +1001,12 @@
         <v>43032</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B65" s="6">
         <v>0</v>
@@ -1021,12 +1015,12 @@
         <v>43032</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B66" s="6">
         <v>0</v>
@@ -1035,12 +1029,12 @@
         <v>43032</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B67" s="6">
         <v>0</v>
@@ -1049,12 +1043,12 @@
         <v>43032</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B68" s="6">
         <v>0</v>
@@ -1063,7 +1057,7 @@
         <v>43032</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modif planning > pop up tuto a intégré, boutique ok
</commit_message>
<xml_diff>
--- a/Docs/Planning.xlsx
+++ b/Docs/Planning.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tentapoulpe\Desktop\TetrisLike\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louis\Desktop\constructor\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="62">
   <si>
     <t>Pourcentage</t>
   </si>
@@ -207,6 +207,9 @@
   </si>
   <si>
     <t>Icone du jeu</t>
+  </si>
+  <si>
+    <t>pop up tuto a intégré</t>
   </si>
 </sst>
 </file>
@@ -246,7 +249,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -277,6 +280,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -290,7 +299,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -302,6 +311,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -618,8 +628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5A1332F-9C89-4503-92BB-2BAE5CF2A291}">
   <dimension ref="A1:D88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="B88" sqref="B88"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="D75" sqref="D75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1086,11 +1096,14 @@
       <c r="A72" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B72" s="6">
-        <v>0</v>
+      <c r="B72" s="11">
+        <v>0.8</v>
       </c>
       <c r="C72" s="5">
         <v>43032</v>
+      </c>
+      <c r="D72" s="8" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
@@ -1179,8 +1192,8 @@
       <c r="A84" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="B84" s="6">
-        <v>0</v>
+      <c r="B84" s="4">
+        <v>1</v>
       </c>
       <c r="C84" s="5">
         <v>43033</v>

</xml_diff>

<commit_message>
plannig + confetti + prefab
</commit_message>
<xml_diff>
--- a/Docs/Planning.xlsx
+++ b/Docs/Planning.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louis\Desktop\constructor\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tentapoulpe\Desktop\TetrisLike\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -249,7 +249,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -280,12 +280,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -299,7 +293,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -311,7 +305,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -628,8 +621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5A1332F-9C89-4503-92BB-2BAE5CF2A291}">
   <dimension ref="A1:D88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="D75" sqref="D75"/>
+    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1007,7 +1000,7 @@
       <c r="A63" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B63" s="6">
+      <c r="B63" s="4">
         <v>0</v>
       </c>
       <c r="C63" s="5">
@@ -1021,7 +1014,7 @@
       <c r="A64" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B64" s="6">
+      <c r="B64" s="4">
         <v>0</v>
       </c>
       <c r="C64" s="5">
@@ -1035,7 +1028,7 @@
       <c r="A65" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B65" s="6">
+      <c r="B65" s="4">
         <v>0</v>
       </c>
       <c r="C65" s="5">
@@ -1049,7 +1042,7 @@
       <c r="A66" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B66" s="6">
+      <c r="B66" s="4">
         <v>0</v>
       </c>
       <c r="C66" s="5">
@@ -1063,7 +1056,7 @@
       <c r="A67" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B67" s="6">
+      <c r="B67" s="4">
         <v>0</v>
       </c>
       <c r="C67" s="5">
@@ -1077,7 +1070,7 @@
       <c r="A68" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B68" s="6">
+      <c r="B68" s="4">
         <v>0</v>
       </c>
       <c r="C68" s="5">
@@ -1096,7 +1089,7 @@
       <c r="A72" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B72" s="11">
+      <c r="B72" s="10">
         <v>0.8</v>
       </c>
       <c r="C72" s="5">
@@ -1203,8 +1196,8 @@
       <c r="A85" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="B85" s="6">
-        <v>0</v>
+      <c r="B85" s="4">
+        <v>1</v>
       </c>
       <c r="C85" s="5">
         <v>43033</v>

</xml_diff>

<commit_message>
Modif scene commencement et kevin confetti
</commit_message>
<xml_diff>
--- a/Docs/Planning.xlsx
+++ b/Docs/Planning.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="65">
   <si>
     <t>Pourcentage</t>
   </si>
@@ -176,9 +176,6 @@
     <t>Prez</t>
   </si>
   <si>
-    <t>FeedBacks :</t>
-  </si>
-  <si>
     <t>Appuyer n'importe ou</t>
   </si>
   <si>
@@ -209,7 +206,19 @@
     <t>Icone du jeu</t>
   </si>
   <si>
-    <t>pop up tuto a intégré</t>
+    <t>FeedBacks et son :</t>
+  </si>
+  <si>
+    <t>Son confetti</t>
+  </si>
+  <si>
+    <t>Son Drag</t>
+  </si>
+  <si>
+    <t>Son Piece rentrée</t>
+  </si>
+  <si>
+    <t>Son bouton (jouer et général)</t>
   </si>
 </sst>
 </file>
@@ -293,7 +302,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -305,6 +314,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -619,10 +629,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5A1332F-9C89-4503-92BB-2BAE5CF2A291}">
-  <dimension ref="A1:D88"/>
+  <dimension ref="A1:D92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="B76" sqref="B76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1007,7 +1017,7 @@
         <v>43032</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
@@ -1021,7 +1031,7 @@
         <v>43032</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
@@ -1035,7 +1045,7 @@
         <v>43032</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
@@ -1049,7 +1059,7 @@
         <v>43032</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
@@ -1063,7 +1073,7 @@
         <v>43032</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
@@ -1077,7 +1087,7 @@
         <v>43032</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
@@ -1089,15 +1099,13 @@
       <c r="A72" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B72" s="10">
-        <v>0.8</v>
+      <c r="B72" s="4">
+        <v>1</v>
       </c>
       <c r="C72" s="5">
         <v>43032</v>
       </c>
-      <c r="D72" s="8" t="s">
-        <v>61</v>
-      </c>
+      <c r="D72" s="8"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="8" t="s">
@@ -1137,7 +1145,7 @@
         <v>49</v>
       </c>
       <c r="B76" s="10">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="C76" s="9">
         <v>43034</v>
@@ -1145,12 +1153,12 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="8" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B81" s="4">
         <v>1</v>
@@ -1161,7 +1169,7 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B82" s="6">
         <v>0</v>
@@ -1172,7 +1180,7 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B83" s="6">
         <v>0</v>
@@ -1183,7 +1191,7 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B84" s="4">
         <v>1</v>
@@ -1194,7 +1202,7 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B85" s="4">
         <v>1</v>
@@ -1205,7 +1213,7 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B86" s="6">
         <v>0</v>
@@ -1216,10 +1224,10 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="B87" s="6">
-        <v>0</v>
+        <v>56</v>
+      </c>
+      <c r="B87" s="4">
+        <v>1</v>
       </c>
       <c r="C87" s="5">
         <v>43033</v>
@@ -1227,13 +1235,57 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="B88" s="6">
-        <v>0</v>
+        <v>59</v>
+      </c>
+      <c r="B88" s="11">
+        <v>0.5</v>
       </c>
       <c r="C88" s="5">
         <v>43033</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A89" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B89" s="4">
+        <v>1</v>
+      </c>
+      <c r="C89" s="5">
+        <v>43034</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A90" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B90" s="6">
+        <v>0</v>
+      </c>
+      <c r="C90" s="5">
+        <v>43034</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A91" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B91" s="6">
+        <v>0</v>
+      </c>
+      <c r="C91" s="5">
+        <v>43034</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A92" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B92" s="6">
+        <v>0</v>
+      </c>
+      <c r="C92" s="5">
+        <v>43034</v>
       </c>
     </row>
   </sheetData>

</xml_diff>